<commit_message>
rerun of both_cleaned file to get agg data
</commit_message>
<xml_diff>
--- a/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_2020.10.09.xlsx
+++ b/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_2020.10.09.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/us_plants_digitization_status/gbif_idigbio_institutionCode_summary_cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AE66213-9340-CC40-A348-5211947618B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676BC18E-1E32-E04D-AC08-FDFAF675C8ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
   </bookViews>
   <sheets>
     <sheet name="gbif" sheetId="1" r:id="rId1"/>
@@ -1831,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC116848-9522-DC4A-A761-05525103B3D5}">
   <dimension ref="A1:AB197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:AB197"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18788,8 +18788,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566BEF74-26DA-4941-9C2C-AB078E807C2E}">
   <dimension ref="A1:AA378"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
small updates to both_cleaned october file
</commit_message>
<xml_diff>
--- a/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_2020.10.09.xlsx
+++ b/gbif_idigbio_institutionCode_summary_cleaned/both_cleaned_2020.10.09.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jocelynpender/us_plants_digitization_status/gbif_idigbio_institutionCode_summary_cleaned/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676BC18E-1E32-E04D-AC08-FDFAF675C8ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE5FB3AF-9121-5E40-B8AF-886E416B7837}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{727722C5-4F6C-E542-A1FA-45A2F6FFAA03}"/>
   </bookViews>
   <sheets>
     <sheet name="gbif" sheetId="1" r:id="rId1"/>
@@ -1831,8 +1831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC116848-9522-DC4A-A761-05525103B3D5}">
   <dimension ref="A1:AB197"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18788,7 +18788,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{566BEF74-26DA-4941-9C2C-AB078E807C2E}">
   <dimension ref="A1:AA378"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>